<commit_message>
first commit from asus
</commit_message>
<xml_diff>
--- a/Valori Turometru.xlsx
+++ b/Valori Turometru.xlsx
@@ -76,13 +76,16 @@
           <c:trendline>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
-            <c:dispRSqr val="1"/>
+          </c:trendline>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.44491951006124236"/>
-                  <c:y val="-0.67643117526975793"/>
+                  <c:x val="0.36697091440705887"/>
+                  <c:y val="-0.63571340040828228"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
@@ -90,23 +93,71 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$5</c:f>
+              <c:f>Sheet1!$A$1:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>318</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>274</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>242</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>210</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="10">
+                  <c:v>187</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>145</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
@@ -114,46 +165,94 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$5</c:f>
+              <c:f>Sheet1!$B$1:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="10">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2780</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>3000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
+                  <c:v>3100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3250</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3450</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3550</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>4000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="55410048"/>
-        <c:axId val="55408512"/>
+        <c:axId val="55137792"/>
+        <c:axId val="55139328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="55410048"/>
+        <c:axId val="55137792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55408512"/>
+        <c:crossAx val="55139328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55408512"/>
+        <c:axId val="55139328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -161,7 +260,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55410048"/>
+        <c:crossAx val="55137792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -174,7 +273,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -204,7 +303,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0.35761876640419948"/>
-                  <c:y val="-4.1156678331875182E-2"/>
+                  <c:y val="-4.1156678331875175E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
@@ -212,7 +311,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$18:$A$24</c:f>
+              <c:f>Sheet1!$A$25:$A$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -242,7 +341,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$18:$B$24</c:f>
+              <c:f>Sheet1!$B$25:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -271,23 +370,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="47558656"/>
-        <c:axId val="75880320"/>
+        <c:axId val="55147520"/>
+        <c:axId val="55161600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47558656"/>
+        <c:axId val="55147520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75880320"/>
+        <c:crossAx val="55161600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75880320"/>
+        <c:axId val="55161600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -295,7 +394,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47558656"/>
+        <c:crossAx val="55147520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -308,7 +407,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -349,15 +448,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -664,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -682,134 +781,256 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>274</v>
+        <v>313</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>210</v>
+        <v>307</v>
       </c>
       <c r="B3">
-        <v>2000</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>145</v>
+        <v>301</v>
       </c>
       <c r="B4">
-        <v>3000</v>
+        <v>390</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>90</v>
+        <v>293</v>
       </c>
       <c r="B5">
-        <v>4000</v>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>284</v>
+      </c>
+      <c r="B6">
+        <v>850</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>318</v>
+        <v>274</v>
       </c>
       <c r="B7">
-        <f>-0.000239*A7^3+A7^2*0.138437-41.005076*A7+6748.5</f>
-        <v>22.562771999999313</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="B8">
-        <f t="shared" ref="B8:B10" si="0">-0.000239*A8^3+A8^2*0.138437-41.005076*A8+6748.5</f>
-        <v>989.9784520000012</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
+        <v>242</v>
+      </c>
+      <c r="B9">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
         <v>210</v>
       </c>
-      <c r="B9">
+      <c r="B10">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>187</v>
+      </c>
+      <c r="B11">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>168</v>
+      </c>
+      <c r="B12">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>155</v>
+      </c>
+      <c r="B13">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>145</v>
+      </c>
+      <c r="B14">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>136</v>
+      </c>
+      <c r="B15">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>128</v>
+      </c>
+      <c r="B16">
+        <v>3250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>122</v>
+      </c>
+      <c r="B17">
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>116</v>
+      </c>
+      <c r="B18">
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>111</v>
+      </c>
+      <c r="B19">
+        <v>3550</v>
+      </c>
+      <c r="G19">
+        <v>318</v>
+      </c>
+      <c r="H19">
+        <f>-0.000239*G19^3+G19^2*0.138437-41.005076*G19+6748.5</f>
+        <v>22.562771999999313</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>106</v>
+      </c>
+      <c r="B20">
+        <v>3700</v>
+      </c>
+      <c r="G20">
+        <v>274</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ref="H20:H22" si="0">-0.000239*G20^3+G20^2*0.138437-41.005076*G20+6748.5</f>
+        <v>989.9784520000012</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>90</v>
+      </c>
+      <c r="B21">
+        <v>4000</v>
+      </c>
+      <c r="G21">
+        <v>210</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>2029.1267400000006</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10">
+    <row r="22" spans="1:8">
+      <c r="G22">
         <v>145</v>
       </c>
-      <c r="B10">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>2984.7805299999995</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11">
+    <row r="23" spans="1:8">
+      <c r="G23">
         <v>90</v>
       </c>
-      <c r="B11">
-        <f>-0.000239*A11^3+A11^2*0.138437-41.005076*A11+6748.5</f>
+      <c r="H23">
+        <f>-0.000239*G23^3+G23^2*0.138437-41.005076*G23+6748.5</f>
         <v>4005.1518599999999</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18">
+    <row r="25" spans="1:8">
+      <c r="A25">
         <v>94</v>
       </c>
-      <c r="B18">
+      <c r="B25">
         <v>4000</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19">
+    <row r="26" spans="1:8">
+      <c r="A26">
         <v>119</v>
       </c>
-      <c r="B19">
+      <c r="B26">
         <v>4500</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20">
+    <row r="27" spans="1:8">
+      <c r="A27">
         <v>154</v>
       </c>
-      <c r="B20">
+      <c r="B27">
         <v>5000</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21">
+    <row r="28" spans="1:8">
+      <c r="A28">
         <v>189</v>
       </c>
-      <c r="B21">
+      <c r="B28">
         <v>5500</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22">
+    <row r="29" spans="1:8">
+      <c r="A29">
         <v>224</v>
       </c>
-      <c r="B22">
+      <c r="B29">
         <v>6000</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23">
+    <row r="30" spans="1:8">
+      <c r="A30">
         <v>254</v>
       </c>
-      <c r="B23">
+      <c r="B30">
         <v>6500</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24">
+    <row r="31" spans="1:8">
+      <c r="A31">
         <v>279</v>
       </c>
-      <c r="B24">
+      <c r="B31">
         <v>7000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
made first 2 steps of first scenario work
</commit_message>
<xml_diff>
--- a/Valori Turometru.xlsx
+++ b/Valori Turometru.xlsx
@@ -148,23 +148,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="56803712"/>
-        <c:axId val="56805248"/>
+        <c:axId val="55154560"/>
+        <c:axId val="55156096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56803712"/>
+        <c:axId val="55154560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56805248"/>
+        <c:crossAx val="55156096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56805248"/>
+        <c:axId val="55156096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -172,20 +172,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56803712"/>
+        <c:crossAx val="55154560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -212,8 +211,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.41087729658792649"/>
-                  <c:y val="-0.66717191601049863"/>
+                  <c:x val="0.41087729658792654"/>
+                  <c:y val="-0.66717191601049886"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
@@ -365,23 +364,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="42513152"/>
-        <c:axId val="42445440"/>
+        <c:axId val="55177600"/>
+        <c:axId val="55179136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42513152"/>
+        <c:axId val="55177600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42445440"/>
+        <c:crossAx val="55179136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42445440"/>
+        <c:axId val="55179136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -389,20 +388,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42513152"/>
+        <c:crossAx val="55177600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -413,11 +411,26 @@
   <c:lang val="en-US"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Stanga: y-&gt;viteza </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.78023600174978114"/>
+          <c:x val="0.78023600174978103"/>
           <c:y val="0.30555555555555558"/>
         </c:manualLayout>
       </c:layout>
@@ -428,9 +441,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0599518810148726E-2"/>
-          <c:y val="2.8252405949256341E-2"/>
-          <c:w val="0.68243503937007877"/>
+          <c:x val="7.059951881014874E-2"/>
+          <c:y val="2.8252405949256338E-2"/>
+          <c:w val="0.68243503937007888"/>
           <c:h val="0.79822506561679785"/>
         </c:manualLayout>
       </c:layout>
@@ -452,7 +465,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.26289260717410323"/>
+                  <c:x val="0.26289260717410334"/>
                   <c:y val="-0.64402376786235049"/>
                 </c:manualLayout>
               </c:layout>
@@ -545,23 +558,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="70964352"/>
-        <c:axId val="42654336"/>
+        <c:axId val="55494144"/>
+        <c:axId val="55495680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="70964352"/>
+        <c:axId val="55494144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42654336"/>
+        <c:crossAx val="55495680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42654336"/>
+        <c:axId val="55495680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,7 +582,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70964352"/>
+        <c:crossAx val="55494144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -582,7 +595,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -597,7 +610,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.80829155730533686"/>
+          <c:x val="0.80829155730533697"/>
           <c:y val="0.30555555555555558"/>
         </c:manualLayout>
       </c:layout>
@@ -719,23 +732,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="56782208"/>
-        <c:axId val="56780288"/>
+        <c:axId val="55660928"/>
+        <c:axId val="55662464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56782208"/>
+        <c:axId val="55660928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56780288"/>
+        <c:crossAx val="55662464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56780288"/>
+        <c:axId val="55662464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +756,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56782208"/>
+        <c:crossAx val="55660928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -756,7 +769,187 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.61946522309711283"/>
+          <c:y val="0.26851851851851855"/>
+        </c:manualLayout>
+      </c:layout>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10134951881014873"/>
+          <c:y val="0.19954870224555263"/>
+          <c:w val="0.50843525809273837"/>
+          <c:h val="0.65007691746864971"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Stanga: viteza-&gt; y</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.14629330708661417"/>
+                  <c:y val="-0.62752952755905511"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Viteza!$L$2:$L$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Viteza!$M$2:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>304</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>72</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="57578240"/>
+        <c:axId val="57523200"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="57578240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="57523200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="57523200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="57578240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -884,6 +1077,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1211,7 +1434,7 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4">
-        <f>M4+21</f>
+        <f t="shared" ref="A4:A21" si="0">M4+21</f>
         <v>322</v>
       </c>
       <c r="B4">
@@ -1223,7 +1446,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5">
-        <f>M5+21</f>
+        <f t="shared" si="0"/>
         <v>314</v>
       </c>
       <c r="B5">
@@ -1235,7 +1458,7 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6">
-        <f>M6+21</f>
+        <f t="shared" si="0"/>
         <v>305</v>
       </c>
       <c r="B6">
@@ -1247,7 +1470,7 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7">
-        <f>M7+21</f>
+        <f t="shared" si="0"/>
         <v>295</v>
       </c>
       <c r="B7">
@@ -1259,7 +1482,7 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8">
-        <f>M8+21</f>
+        <f t="shared" si="0"/>
         <v>282</v>
       </c>
       <c r="B8">
@@ -1271,7 +1494,7 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9">
-        <f>M9+21</f>
+        <f t="shared" si="0"/>
         <v>263</v>
       </c>
       <c r="B9">
@@ -1283,7 +1506,7 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10">
-        <f>M10+21</f>
+        <f t="shared" si="0"/>
         <v>231</v>
       </c>
       <c r="B10">
@@ -1295,7 +1518,7 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11">
-        <f>M11+21</f>
+        <f t="shared" si="0"/>
         <v>208</v>
       </c>
       <c r="B11">
@@ -1307,7 +1530,7 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12">
-        <f>M12+21</f>
+        <f t="shared" si="0"/>
         <v>189</v>
       </c>
       <c r="B12">
@@ -1319,7 +1542,7 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13">
-        <f>M13+21</f>
+        <f t="shared" si="0"/>
         <v>176</v>
       </c>
       <c r="B13">
@@ -1331,7 +1554,7 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14">
-        <f>M14+21</f>
+        <f t="shared" si="0"/>
         <v>166</v>
       </c>
       <c r="B14">
@@ -1343,7 +1566,7 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15">
-        <f>M15+21</f>
+        <f t="shared" si="0"/>
         <v>157</v>
       </c>
       <c r="B15">
@@ -1355,7 +1578,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16">
-        <f>M16+21</f>
+        <f t="shared" si="0"/>
         <v>149</v>
       </c>
       <c r="B16">
@@ -1367,7 +1590,7 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17">
-        <f>M17+21</f>
+        <f t="shared" si="0"/>
         <v>143</v>
       </c>
       <c r="B17">
@@ -1379,7 +1602,7 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18">
-        <f>M18+21</f>
+        <f t="shared" si="0"/>
         <v>137</v>
       </c>
       <c r="B18">
@@ -1391,7 +1614,7 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19">
-        <f>M19+21</f>
+        <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="B19">
@@ -1410,7 +1633,7 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20">
-        <f>M20+21</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="B20">
@@ -1420,7 +1643,7 @@
         <v>274</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:H22" si="0">-0.000239*G20^3+G20^2*0.138437-41.005076*G20+6748.5</f>
+        <f t="shared" ref="H20:H22" si="1">-0.000239*G20^3+G20^2*0.138437-41.005076*G20+6748.5</f>
         <v>989.9784520000012</v>
       </c>
       <c r="M20">
@@ -1429,7 +1652,7 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21">
-        <f>M21+21</f>
+        <f t="shared" si="0"/>
         <v>111</v>
       </c>
       <c r="B21">
@@ -1439,7 +1662,7 @@
         <v>210</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2029.1267400000006</v>
       </c>
       <c r="M21">
@@ -1451,7 +1674,7 @@
         <v>145</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2984.7805299999995</v>
       </c>
     </row>
@@ -1528,15 +1751,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:14">
       <c r="A1">
         <v>349</v>
       </c>
@@ -1544,84 +1767,196 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>326</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>N2-45</f>
+        <v>304</v>
+      </c>
+      <c r="N2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>304</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <f>N3-45</f>
+        <v>281</v>
+      </c>
+      <c r="N3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>279</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="L4">
+        <v>15</v>
+      </c>
+      <c r="M4">
+        <f>N4-45</f>
+        <v>259</v>
+      </c>
+      <c r="N4">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>254</v>
       </c>
       <c r="B5">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="L5">
+        <v>20</v>
+      </c>
+      <c r="M5">
+        <f>N5-45</f>
+        <v>234</v>
+      </c>
+      <c r="N5">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>230</v>
       </c>
       <c r="B6">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="L6">
+        <v>25</v>
+      </c>
+      <c r="M6">
+        <f>N6-45</f>
+        <v>209</v>
+      </c>
+      <c r="N6">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>208</v>
       </c>
       <c r="B7">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="L7">
+        <v>30</v>
+      </c>
+      <c r="M7">
+        <f>N7-45</f>
+        <v>185</v>
+      </c>
+      <c r="N7">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>181</v>
       </c>
       <c r="B8">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="L8">
+        <v>34</v>
+      </c>
+      <c r="M8">
+        <f>N8-45</f>
+        <v>163</v>
+      </c>
+      <c r="N8">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>157</v>
       </c>
       <c r="B9">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="L9">
+        <v>40</v>
+      </c>
+      <c r="M9">
+        <f>N9-45</f>
+        <v>136</v>
+      </c>
+      <c r="N9">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10">
         <v>136</v>
       </c>
       <c r="B10">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="L10">
+        <v>45</v>
+      </c>
+      <c r="M10">
+        <f>N10-45</f>
+        <v>112</v>
+      </c>
+      <c r="N10">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>117</v>
       </c>
       <c r="B11">
         <v>55</v>
+      </c>
+      <c r="L11">
+        <v>50</v>
+      </c>
+      <c r="M11">
+        <f>N11-45</f>
+        <v>91</v>
+      </c>
+      <c r="N11">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="L12">
+        <v>55</v>
+      </c>
+      <c r="M12">
+        <f>N12-45</f>
+        <v>72</v>
+      </c>
+      <c r="N12">
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:2">

</xml_diff>